<commit_message>
get tables, some fixes for right coords
</commit_message>
<xml_diff>
--- a/ahihi.xlsx
+++ b/ahihi.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -340,7 +341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -356,307 +357,179 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>0.2435342347303546</v>
+        <v>-1.292080721726155</v>
       </c>
       <c r="B2">
-        <v>40.09477457100703</v>
+        <v>40.47579836825359</v>
       </c>
       <c r="E2">
-        <v>-30.14</v>
+        <v>-29.97</v>
       </c>
       <c r="F2">
-        <v>18.77</v>
+        <v>19.93</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>-31.39610802037789</v>
+        <v>-32.37101184192168</v>
       </c>
       <c r="B3">
-        <v>17.99228803524018</v>
+        <v>18.50804372641845</v>
       </c>
       <c r="E3">
-        <v>-30.2</v>
+        <v>-30.1</v>
       </c>
       <c r="F3">
-        <v>18.69</v>
+        <v>19.53</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>-31.38826016735443</v>
+        <v>-32.354482725765</v>
       </c>
       <c r="B4">
-        <v>17.98915497457645</v>
+        <v>18.735814354647</v>
       </c>
       <c r="E4">
-        <v>-30.28</v>
+        <v>-29.95</v>
       </c>
       <c r="F4">
-        <v>18.63</v>
+        <v>20.03</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>-31.39396038252121</v>
+        <v>-32.3063168398515</v>
       </c>
       <c r="B5">
-        <v>17.88166358628315</v>
+        <v>18.98166524023402</v>
       </c>
       <c r="E5">
-        <v>-30.21</v>
+        <v>-30.06</v>
       </c>
       <c r="F5">
-        <v>18.9</v>
+        <v>19.58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>-31.32018032212796</v>
+        <v>-32.35458014444087</v>
       </c>
       <c r="B6">
-        <v>18.70941523330432</v>
+        <v>18.94176099632543</v>
       </c>
       <c r="E6">
-        <v>-30.21</v>
+        <v>-30.04</v>
       </c>
       <c r="F6">
-        <v>18.9</v>
+        <v>19.76</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>-31.24290945196988</v>
+        <v>-32.31753401087381</v>
       </c>
       <c r="B7">
-        <v>18.61223721366908</v>
+        <v>18.8663606345545</v>
       </c>
       <c r="E7">
-        <v>-30.26</v>
+        <v>-30</v>
       </c>
       <c r="F7">
-        <v>18.81</v>
+        <v>19.88</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>-31.33903496312236</v>
+        <v>-32.3397456370814</v>
       </c>
       <c r="B8">
-        <v>18.67880329769473</v>
+        <v>18.99823253596354</v>
       </c>
       <c r="E8">
-        <v>-30.25</v>
+        <v>-30.07</v>
       </c>
       <c r="F8">
-        <v>18.75</v>
+        <v>19.57</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>-31.32280127491542</v>
+        <v>-32.3719895303408</v>
       </c>
       <c r="B9">
-        <v>18.69093490375297</v>
+        <v>18.57676856475656</v>
       </c>
       <c r="E9">
-        <v>-30.25</v>
+        <v>-29.96</v>
       </c>
       <c r="F9">
-        <v>18.76</v>
+        <v>20.16</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>-31.23228981277464</v>
+        <v>-32.28325829338218</v>
       </c>
       <c r="B10">
-        <v>18.74527511883717</v>
+        <v>19.41418914595164</v>
       </c>
       <c r="E10">
-        <v>-30.23</v>
+        <v>-30.09</v>
       </c>
       <c r="F10">
-        <v>18.79</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>-31.33915902645404</v>
+        <v>-32.26272399813831</v>
       </c>
       <c r="B11">
-        <v>18.64771533331836</v>
+        <v>19.45634640586082</v>
       </c>
       <c r="E11">
-        <v>-30.22</v>
+        <v>-30.15</v>
       </c>
       <c r="F11">
-        <v>18.88</v>
+        <v>19.66</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>-31.34953727001356</v>
+        <v>-32.27723217532559</v>
       </c>
       <c r="B12">
-        <v>18.74731897879122</v>
+        <v>19.50693954850279</v>
       </c>
       <c r="E12">
-        <v>-30.22</v>
+        <v>-30.19</v>
       </c>
       <c r="F12">
-        <v>18.72</v>
+        <v>19.6</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>-31.38040471006295</v>
+        <v>-32.27415980015615</v>
       </c>
       <c r="B13">
-        <v>18.42442347129475</v>
-      </c>
-      <c r="E13">
-        <v>-30.2</v>
-      </c>
-      <c r="F13">
-        <v>18.91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>-31.3333292019266</v>
-      </c>
-      <c r="B14">
-        <v>18.70501838288671</v>
-      </c>
-      <c r="E14">
-        <v>-30.21</v>
-      </c>
-      <c r="F14">
-        <v>18.67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>-31.30552147548754</v>
-      </c>
-      <c r="B15">
-        <v>18.37258624328359</v>
-      </c>
-      <c r="E15">
-        <v>-30.27</v>
-      </c>
-      <c r="F15">
-        <v>18.57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>-31.34114852113672</v>
-      </c>
-      <c r="B16">
-        <v>18.94543987796177</v>
-      </c>
-      <c r="E16">
-        <v>-30.31</v>
-      </c>
-      <c r="F16">
-        <v>18.43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>-31.34575399743903</v>
-      </c>
-      <c r="B17">
-        <v>18.82844365608135</v>
-      </c>
-      <c r="E17">
-        <v>-30.38</v>
-      </c>
-      <c r="F17">
-        <v>18.31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>-31.33975781528644</v>
-      </c>
-      <c r="B18">
-        <v>18.69559518689445</v>
-      </c>
-      <c r="E18">
-        <v>-30.32</v>
-      </c>
-      <c r="F18">
-        <v>18.57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>-31.29829758035923</v>
-      </c>
-      <c r="B19">
-        <v>19.17048788545989</v>
-      </c>
-      <c r="E19">
-        <v>-30.33</v>
-      </c>
-      <c r="F19">
-        <v>18.62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>-31.19827032209295</v>
-      </c>
-      <c r="B20">
-        <v>19.23830486000621</v>
-      </c>
-      <c r="E20">
-        <v>-30.34</v>
-      </c>
-      <c r="F20">
-        <v>18.53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>-31.21910171637379</v>
-      </c>
-      <c r="B21">
-        <v>19.68583076249773</v>
-      </c>
-      <c r="E21">
-        <v>-30.37</v>
-      </c>
-      <c r="F21">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>-31.19122487206244</v>
-      </c>
-      <c r="B22">
-        <v>19.86982637689983</v>
-      </c>
-      <c r="E22">
-        <v>-30.33</v>
-      </c>
-      <c r="F22">
-        <v>18.78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>-28.31657238000478</v>
-      </c>
-      <c r="B23">
-        <v>27.40269790344072</v>
+        <v>19.35380986947552</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>